<commit_message>
divide drinks into different categories
</commit_message>
<xml_diff>
--- a/wine2.xlsx
+++ b/wine2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Илья\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79870\projects\Devman\WebsiteLayout\WMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1B18A6-D0D5-46C6-8795-EDD6EAD4D101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA2D6A9-15D7-4D07-A9D1-05FFFB667314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -399,19 +399,19 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -428,7 +428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -460,7 +460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -477,7 +477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -494,7 +494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -511,7 +511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -528,7 +528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -545,7 +545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -560,7 +560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>